<commit_message>
Code added latest in WFMHomePage
</commit_message>
<xml_diff>
--- a/Data/WFM-ESS Availability Pattern Requests and Manager Approval.xlsx
+++ b/Data/WFM-ESS Availability Pattern Requests and Manager Approval.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{057AFA1A-BC5C-44E3-B697-09700CC2A9AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C15FEE7-C858-4ECD-A7EB-9C80C9C87642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -531,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>

</xml_diff>